<commit_message>
tableau des taches, manque les marge
</commit_message>
<xml_diff>
--- a/Tableau_Des_Taches.xlsx
+++ b/Tableau_Des_Taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Cegep\Session 5 Informatique\PE\DeGuiWii\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8A4DB9-AF3D-4DDA-9955-A2CEE2619D30}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1369263-26E2-4D5C-BBA8-F89E091EB6DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{EE72E57F-06F0-4D34-A1EE-153CBC309DE4}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
   <si>
     <t>No. Tâche</t>
   </si>
@@ -38,9 +38,6 @@
     <t>Tâche</t>
   </si>
   <si>
-    <t>Temps</t>
-  </si>
-  <si>
     <t>Préalable</t>
   </si>
   <si>
@@ -137,15 +134,6 @@
     <t>6.0</t>
   </si>
   <si>
-    <t>6.1</t>
-  </si>
-  <si>
-    <t>6.2</t>
-  </si>
-  <si>
-    <t>6.3</t>
-  </si>
-  <si>
     <t>7.0</t>
   </si>
   <si>
@@ -171,13 +159,22 @@
   </si>
   <si>
     <t>1.0 - 2.0 - 3.0 - 4.0 - 5.0 - 6.0</t>
+  </si>
+  <si>
+    <t>Temps (H)</t>
+  </si>
+  <si>
+    <t>Gestion des Employés</t>
+  </si>
+  <si>
+    <t>TABLEAU DES TÂCHES POUR CO-ECO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,8 +202,23 @@
       <name val="Agency FB"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="Agency FB"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -231,8 +243,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0FD722"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -376,14 +394,118 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -392,7 +514,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -412,9 +534,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -423,7 +543,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -434,7 +553,25 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,6 +580,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF0FD722"/>
       <color rgb="FFEA0000"/>
       <color rgb="FFBC0000"/>
       <color rgb="FFBFB1B1"/>
@@ -760,300 +898,449 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5625688F-58E9-45F0-9A36-7F0BAA0E0980}">
-  <dimension ref="C4:G25"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C5" s="16" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="21"/>
+    </row>
+    <row r="2" spans="1:7" ht="33" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="22"/>
+      <c r="B2" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="23"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="22"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="23"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="22"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="23"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="22"/>
+      <c r="B5" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="C5" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="D5" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="23"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="22"/>
+      <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="23"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="22"/>
+      <c r="B7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="5">
+        <v>10</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="23"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="22"/>
+      <c r="B8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="2">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="23"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="22"/>
+      <c r="B9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="5">
+        <v>10</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="23"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="22"/>
+      <c r="B10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="2">
+        <v>20</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="23"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="B11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="5">
+        <v>20</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="23"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
+      <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="2">
+        <v>15</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="23"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="22"/>
+      <c r="B13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="5">
+        <v>8</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="7"/>
+      <c r="G13" s="23"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="22"/>
+      <c r="B14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="5">
+        <v>2</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="23"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
+      <c r="B15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="5">
         <v>5</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="7"/>
+      <c r="G15" s="23"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="22"/>
+      <c r="B16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="2">
+        <v>10</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="23"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="22"/>
+      <c r="B17" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="5">
         <v>8</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2" t="s">
+      <c r="E17" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="7"/>
+      <c r="G17" s="23"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="22"/>
+      <c r="B18" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="5">
+        <v>2</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="7"/>
+      <c r="G18" s="23"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="22"/>
+      <c r="B19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="2">
+        <v>15</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="8"/>
+      <c r="G19" s="23"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="22"/>
+      <c r="B20" s="4">
+        <v>6.1</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="1" t="s">
+      <c r="D20" s="5">
+        <v>8</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="F20" s="7"/>
+      <c r="G20" s="23"/>
+      <c r="I20" s="28"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="22"/>
+      <c r="B21" s="4">
+        <v>6.2</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="5">
+        <v>2</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="7"/>
+      <c r="G21" s="23"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="22"/>
+      <c r="B22" s="4">
+        <v>6.3</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="5">
+        <v>3</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="7"/>
+      <c r="G22" s="23"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="22"/>
+      <c r="B23" s="4">
+        <v>6.4</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="5">
+        <v>2</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="23"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="22"/>
+      <c r="B24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="2">
+        <v>10</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" s="9"/>
+      <c r="G24" s="23"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="22"/>
+      <c r="B25" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="5">
+        <v>4</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F25" s="7"/>
+      <c r="G25" s="23"/>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="22"/>
+      <c r="B26" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G10" s="10"/>
-    </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G12" s="10"/>
-    </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C13" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G13" s="8"/>
-    </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C14" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G14" s="8"/>
-    </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C15" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="5" t="s">
+      <c r="C26" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" s="8"/>
-    </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G16" s="10"/>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G17" s="8"/>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="5" t="s">
+      <c r="D26" s="11">
         <v>6</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G19" s="19"/>
-    </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G20" s="8"/>
-    </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G21" s="8"/>
-    </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G22" s="8"/>
-    </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" s="9"/>
-      <c r="F23" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G23" s="11"/>
-    </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="4" t="s">
+      <c r="E26" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G24" s="8"/>
-    </row>
-    <row r="25" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E25" s="14"/>
-      <c r="F25" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G25" s="15"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="23"/>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="25"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="27"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:F2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>